<commit_message>
10 steps from ALU to CPU
</commit_message>
<xml_diff>
--- a/xetroc.xlsx
+++ b/xetroc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08e9d1d1b3ac9846/Lehre/RO MPT ES/RO/xetroc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{1DFA63E7-D0C4-4296-8A41-B08683187CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{816B45D5-372A-4CFA-963A-F64580F2200F}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{1DFA63E7-D0C4-4296-8A41-B08683187CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{225ECD2D-395E-4BB6-B859-38290EDDDA9A}"/>
   <bookViews>
-    <workbookView xWindow="42780" yWindow="3210" windowWidth="31830" windowHeight="16455" xr2:uid="{0C8C6F34-8F7C-4CD6-92D1-3EA217BDBAC0}"/>
+    <workbookView xWindow="44235" yWindow="4215" windowWidth="31830" windowHeight="16455" xr2:uid="{0C8C6F34-8F7C-4CD6-92D1-3EA217BDBAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="120">
   <si>
     <t>16-bit encoding</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>self loop, unconditional</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -901,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EA7711-5FD7-475F-9214-D56844A47F92}">
   <dimension ref="B2:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1624,7 @@
         <v>117</v>
       </c>
       <c r="Y14" s="20" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="Z14" s="20">
         <v>-2</v>

</xml_diff>

<commit_message>
bugfix: FlagW were swapped
</commit_message>
<xml_diff>
--- a/xetroc.xlsx
+++ b/xetroc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08e9d1d1b3ac9846/Lehre/RO MPT ES/RO/xetroc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="985" documentId="8_{1DFA63E7-D0C4-4296-8A41-B08683187CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C77977A-7F69-4E3E-AD1F-A456D4479F57}"/>
+  <xr:revisionPtr revIDLastSave="987" documentId="8_{1DFA63E7-D0C4-4296-8A41-B08683187CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B1FA20-7A78-4926-97AC-4FA47582A9F0}"/>
   <bookViews>
-    <workbookView xWindow="20985" yWindow="3000" windowWidth="63615" windowHeight="17880" xr2:uid="{0C8C6F34-8F7C-4CD6-92D1-3EA217BDBAC0}"/>
+    <workbookView xWindow="13185" yWindow="3000" windowWidth="63615" windowHeight="17880" xr2:uid="{0C8C6F34-8F7C-4CD6-92D1-3EA217BDBAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:AM82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:R14"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1593,7 @@
         <v>54</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7" t="s">
@@ -1903,7 +1903,7 @@
         <v>39</v>
       </c>
       <c r="AG8" s="67" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AH8" s="67"/>
       <c r="AI8" s="67">
@@ -3490,7 +3490,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="AC13:AC14 AG13:AG14 A8:P8 A11:P14 A5:J7 A10:E10 A9:E9 I9:P9 I10:P10 A4" numberStoredAsText="1"/>
+    <ignoredError sqref="AC13:AC14 AG13:AG14 A8:P8 A11:P14 A5:J7 A10:E10 A9:E9 I9:P9 I10:P10 A4 AG5:AG12 X5:X14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>